<commit_message>
refactor: update model version to gpt-4o across multiple agents and remove unused main script
</commit_message>
<xml_diff>
--- a/project_context/consolidated_reports.xlsx
+++ b/project_context/consolidated_reports.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,7 +516,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>C:\Users\risha\Downloads\project_context\ppt\2025CodingPirates - YASH KASAUDHAN.pdf</t>
+          <t>D:\hackathon-evaluation\hackathon-evaluation\project_context\ppt\2025CodingPirates - YASH KASAUDHAN.pdf</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -545,48 +545,48 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>The project presents a digital platform aimed at showcasing and preserving the cultural heritage of Sikkim's monasteries. While the concept is strong, the evidence provided lacks critical diagrams and metrics to substantiate claims. The architecture is outlined but lacks detailed scalability and cost estimates. The risks and mitigations are mentioned but not thoroughly analyzed. Overall, the proposal is adequate but has multiple gaps in evidence and clarity.</t>
+          <t>The project by Coding Pirates aims to digitize and showcase the monasteries of Sikkim for tourism and cultural preservation. The deck provides a comprehensive overview of the problem and the proposed solution, including a detailed technical architecture. However, there are gaps in baseline data, cost estimates, and security considerations. The project demonstrates strong potential impact and a clear adoption path, but lacks detailed metrics and evaluation plans.</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>No diagrams were provided to illustrate the workflow or architecture of the project. The absence of visual evidence limits the understanding of the proposed system's functionality and integration.</t>
+          <t>The workflow involves creating a digital platform for virtual tours and cultural preservation of Sikkim's monasteries. It includes a frontend for user interaction, a backend for data management, and AI components for enhanced search capabilities.</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>1. The concept of digitizing and showcasing monasteries is innovative and addresses a significant cultural preservation need. 2. The use of modern technologies like AI and 360° content is commendable and aligns well with current trends in tourism.</t>
+          <t>1. The project addresses a significant cultural and tourism challenge with a well-defined problem statement. 2. The technical architecture is robust and leverages mature technologies, which enhances feasibility.</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>1. The lack of diagrams or visual representations makes it difficult to assess the architecture and workflow of the proposed solution. 2. Many claims regarding feasibility and impact are made without supporting metrics or evidence.</t>
+          <t>1. The deck lacks detailed baseline data and cost estimates, which are crucial for assessing the project's viability. 2. Security considerations are minimally addressed, posing potential risks.</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>1. The tech stack is well-chosen, but more details on how the components will interact and scale are needed. 2. The proposal mentions using AI for image recognition but lacks specifics on the models and datasets to be used.</t>
+          <t>1. The use of React, Node.js, and PostGIS is appropriate for the project's requirements, ensuring scalability and performance. 2. The AI components for image recognition and NLP search are well-integrated but require further validation.</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>1. Include diagrams that illustrate the system architecture, user flow, and data management processes. 2. Provide clear metrics and KPIs to evaluate the project's success and impact on tourism and cultural preservation.</t>
+          <t>1. Include detailed metrics and evaluation plans to measure the project's success effectively. 2. Enhance the security framework to protect user data and ensure compliance with data protection laws.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Algo Wizards</t>
+          <t>ALT_F4</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>C:\Users\risha\Downloads\project_context\ppt\Algo wizards - LAXMI gla.pdf</t>
+          <t>D:\hackathon-evaluation\hackathon-evaluation\project_context\ppt\ALT_f4 - VAIBHAV KUMAR.pdf</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" t="n">
         <v>6</v>
@@ -595,7 +595,7 @@
         <v>6</v>
       </c>
       <c r="G3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H3" t="n">
         <v>5</v>
@@ -604,237 +604,567 @@
         <v>7</v>
       </c>
       <c r="J3" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K3" t="n">
-        <v>58.5</v>
+        <v>54</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>The proposal addresses significant challenges faced by farmers in India, particularly in accessing timely and accurate agricultural advice. However, it lacks detailed metrics for success, a comprehensive evaluation plan, and a clear deployment strategy. The architecture is modular and scalable, but the absence of diagrams limits the clarity of the proposed solution.</t>
+          <t>The team proposes an AI-driven chatbot for public health awareness, focusing on disease prevention and multilingual support. The solution leverages NLP and ML models, integrating trusted medical data sources. While the idea is innovative, the presentation lacks detailed metrics, baselines, and a comprehensive evaluation plan. The architecture and scalability are addressed at a high level, but specifics on latency, cost, and security are minimal.</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>The workflow involves a voice/text/image input from farmers, which is processed through various stages including preprocessing, AI engine processing, and advisory generation, ultimately delivering outputs in local languages. However, the lack of diagrams means the workflow is not visually represented, which could enhance understanding.</t>
+          <t>No diagrams were provided, so the workflow is inferred from the text. The process involves data collection, preprocessing, NLP model training, chatbot integration, and deployment. The chatbot is designed to be multilingual and continuously learns from user feedback.</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>1. The solution effectively addresses a critical issue in agriculture by leveraging AI to provide timely advice. 2. The use of multilingual NLP is a strong feature that enhances accessibility for non-literate users. 3. The modular architecture allows for scalability across different regions and languages.</t>
+          <t>1. The integration of AI with vernacular language support is a strong point, addressing a significant need in diverse linguistic regions. 2. The use of trusted medical data sources enhances the credibility of the chatbot.</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>1. The proposal lacks concrete metrics and KPIs to measure the success of the solution. 2. There is insufficient detail on the evaluation plan and how the effectiveness of the advisory system will be assessed. 3. The absence of diagrams makes it difficult to visualize the architecture and workflow.</t>
+          <t>1. The presentation lacks diagrams, which makes it difficult to visualize the architecture and workflow. 2. There is insufficient detail on the evaluation plan and metrics to measure success.</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>1. The technical stack is well-defined, but more information on the integration of various APIs and how they interact with the AI engine would be beneficial. 2. Consideration of latency and cost estimates for the deployment of the system is missing.</t>
+          <t>1. The choice of technologies like TensorFlow/PyTorch and cloud deployment is appropriate, but more details on the specific architecture would be beneficial. 2. The security and privacy aspects are not thoroughly addressed, which is critical for handling sensitive health data.</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>1. Include diagrams to visually represent the architecture and workflow, which would clarify the proposed solution. 2. Develop a detailed evaluation plan with specific metrics to assess the impact of the advisory system on farmers' productivity and income. 3. Address potential risks and mitigations related to data privacy and security.</t>
+          <t>1. Include detailed diagrams to illustrate the architecture and workflow. 2. Provide a comprehensive evaluation plan with clear metrics and baselines. 3. Address security and privacy concerns more thoroughly, possibly with a dedicated section on compliance with health data regulations.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AlgoYoddhas</t>
+          <t>Kairos</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>C:\Users\risha\Downloads\project_context\ppt\AlgoYoddhas - ADWAIT PATEL.pdf</t>
+          <t>D:\hackathon-evaluation\hackathon-evaluation\project_context\ppt\AgriNiti - TEENA gla.pdf</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G4" t="n">
         <v>4</v>
       </c>
       <c r="H4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I4" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J4" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="K4" t="n">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>The proposal outlines a mobile and web platform for crowdsourced ocean hazard reporting, integrating social media analytics. While it presents a feasible solution with some innovative elements, it lacks detailed metrics, a comprehensive evaluation plan, and clear architecture diagrams. The absence of critical diagrams limits the overall clarity and robustness of the proposal.</t>
+          <t>The team Kairos presents a solution aimed at empowering small and marginal farmers through an AI-driven crop advisory system. The solution integrates soil, climate, and market data to provide crop recommendations, pest and disease detection, and localized weather alerts. The approach leverages standard web technologies and government APIs, with a focus on accessibility through a multilingual mobile app. However, the presentation lacks detailed diagrams and metrics, and the assumptions and baselines are not well-defined.</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>The workflow is centered around a mobile and web platform that allows users to report hazards in real-time, leveraging NLP for data analysis. However, without diagrams, the workflow lacks visual clarity and detailed architecture.</t>
+          <t>No diagrams were provided, so the workflow could not be analyzed.</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>The concept of integrating crowdsourced data with social media analytics is innovative and addresses a critical need in disaster management. The focus on multilingual and offline capabilities is commendable, especially for remote areas.</t>
+          <t>1. The solution addresses a significant problem for small and marginal farmers, aiming to increase income and reduce crop loss. 2. The use of AI for crop recommendations and pest detection is innovative and has the potential for high impact.</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>The proposal lacks detailed diagrams that could illustrate the architecture and workflow, making it difficult to assess the technical feasibility fully. Additionally, the claims regarding faster response times and citizen participation need more substantiation.</t>
+          <t>1. The presentation lacks detailed diagrams, which makes it difficult to assess the technical feasibility and architecture of the solution. 2. There is insufficient evidence of a well-defined evaluation plan or metrics to measure success.</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>While the use of open-source GIS and NLP tools is a strong point, the proposal does not provide sufficient detail on the data verification process or how the AI filters will be implemented. More technical specifics are needed to evaluate scalability and security.</t>
+          <t>1. The integration with existing government APIs is a strong point, but the scalability and latency of the system are not addressed. 2. The use of standard web technologies is appropriate, but more details on the backend architecture are needed.</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>Include diagrams to illustrate the system architecture and workflow. Provide clearer metrics and KPIs to support claims of impact. Consider detailing the data verification process and how the platform will handle fake reports more comprehensively.</t>
+          <t>1. Include detailed diagrams to illustrate the system architecture and data flow. 2. Define clear metrics and an evaluation plan to measure the impact and success of the solution. 3. Address potential risks and provide mitigation strategies, especially concerning data privacy and security.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BrajCoders</t>
+          <t>Algo Wizards</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>C:\Users\risha\Downloads\project_context\ppt\BrajCoders - DEEPTI YADAV.pdf</t>
+          <t>D:\hackathon-evaluation\hackathon-evaluation\project_context\ppt\Algo wizards - LAXMI gla.pdf</t>
         </is>
       </c>
       <c r="D5" t="n">
         <v>6</v>
       </c>
       <c r="E5" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" t="n">
+        <v>6</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I5" t="n">
         <v>7</v>
       </c>
-      <c r="F5" t="n">
-        <v>7</v>
-      </c>
-      <c r="G5" t="n">
-        <v>5</v>
-      </c>
-      <c r="H5" t="n">
-        <v>6</v>
-      </c>
-      <c r="I5" t="n">
-        <v>8</v>
-      </c>
       <c r="J5" t="n">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K5" t="n">
-        <v>65.5</v>
+        <v>58.5</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>The proposal outlines a low-cost IoT system for monitoring renewable energy in rural areas, emphasizing its affordability, user-friendliness, and predictive maintenance capabilities. However, the lack of diagrams and concrete metrics limits the overall strength of the submission. While the text provides a reasonable overview of the project's feasibility and potential impact, critical areas such as architecture, datasets, and cost estimates are inadequately addressed.</t>
+          <t>Algo Wizards present an AI-based Farmer Query Support and Advisory System aimed at addressing the challenges faced by farmers in accessing real-time, accurate advice. The solution leverages multilingual NLP and voice-based interaction to break language barriers and provide instant, expert-level guidance. While the problem is well-framed and the solution innovative, the deck lacks detailed baselines, metrics, and a comprehensive evaluation plan. The architecture is modular, allowing scalability, but lacks detailed latency and cost estimates. Privacy, compliance, and security considerations are minimally addressed.</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>No diagrams were provided to analyze the workflow of the proposed system. The absence of visual representations limits the understanding of the architecture and operational flow.</t>
+          <t>The workflow involves farmers submitting queries via voice, text, or image, which are then preprocessed and analyzed by an AI engine. The system generates advisory outputs in local languages, providing guidance on crop diseases, fertilizer recommendations, weather-based irrigation, and government schemes.</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>1. The concept of a low-cost IoT system for renewable energy monitoring is innovative and addresses a significant need in rural areas. 2. The focus on user-friendly mobile applications in local languages is commendable and enhances accessibility. 3. The potential social and economic impacts outlined are promising and relevant.</t>
+          <t>1. The solution effectively addresses language barriers and accessibility issues for non-literate users through multilingual NLP and voice-based interaction. 2. The modular architecture allows for easy scaling across different regions and crop types.</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>1. The absence of diagrams or visual aids makes it difficult to assess the architecture and workflow of the proposed system. 2. Key areas such as latency and cost estimates are not addressed, which raises concerns about the project's feasibility. 3. The claims regarding impact metrics lack supporting data or references.</t>
+          <t>1. The deck lacks detailed baselines and metrics to evaluate the effectiveness of the solution. 2. Privacy, compliance, and security considerations are not adequately addressed.</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>1. The tech stack mentioned is diverse but lacks clarity on how these components will integrate effectively. 2. More detailed information on the data collection methods and analysis processes is needed to validate the claims of predictive maintenance and energy loss identification.</t>
+          <t>1. The technical stack is well-defined, but the absence of latency and cost estimates raises concerns about the feasibility of large-scale deployment. 2. The use of APIs for weather, government schemes, and translation is a strong point, but the integration details are not provided.</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>1. Include diagrams that illustrate the system architecture and data flow to enhance understanding. 2. Provide concrete metrics and KPIs to support claims of impact and feasibility. 3. Address potential risks and mitigation strategies in more detail, particularly regarding connectivity and user adoption.</t>
+          <t>1. Include detailed baselines and metrics to measure the impact and effectiveness of the solution. 2. Address privacy, compliance, and security concerns to ensure user trust and data protection. 3. Provide latency and cost estimates to assess the feasibility of scaling the solution.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Caffeinated Coders</t>
+          <t>AlgoYoddhas</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>C:\Users\risha\Downloads\project_context\ppt\Caffeinated Coders - Rohnish Srivastava.pdf</t>
+          <t>D:\hackathon-evaluation\hackathon-evaluation\project_context\ppt\AlgoYoddhas - ADWAIT PATEL.pdf</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="n">
+        <v>4</v>
+      </c>
+      <c r="G6" t="n">
+        <v>4</v>
+      </c>
+      <c r="H6" t="n">
+        <v>5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>6</v>
+      </c>
+      <c r="J6" t="n">
+        <v>28</v>
+      </c>
+      <c r="K6" t="n">
+        <v>46</v>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>The AlgoYoddhas team proposes a mobile and web platform for crowdsourced ocean hazard reporting, integrating social media analytics. The solution includes geotagged reports, a real-time dashboard, and an NLP engine for sentiment analysis. While the proposal outlines a feasible approach using open-source GIS and NLP tools, it lacks detailed diagrams and metrics. The team identifies challenges such as data verification and limited connectivity, offering solutions like role-based access and AI filters. However, the absence of diagrams and specific metrics limits the evaluation of their technical approach and scalability.</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>No diagrams were provided, so the workflow analysis is based solely on the text description. The proposed workflow involves users submitting geotagged reports, which are then analyzed by an NLP engine and displayed on a real-time dashboard. The platform supports multilingual and offline capabilities, aiming to enhance situational awareness and response times.</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>1. The platform addresses a critical need for real-time hazard reporting and social media analytics in disaster management. 2. The use of open-source GIS and NLP tools is a practical approach to ensure feasibility and cost-effectiveness.</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>1. The proposal lacks detailed diagrams, which makes it difficult to fully understand the technical architecture and workflow. 2. There is insufficient information on the datasets and baselines used for the NLP engine.</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>1. The absence of latency and cost estimates raises concerns about the platform's scalability and performance in real-world scenarios. 2. The security and privacy compliance aspects are not adequately addressed, which are critical for handling sensitive data.</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>1. Include detailed architecture diagrams to better illustrate the technical workflow and system components. 2. Provide specific metrics and KPIs to evaluate the platform's effectiveness and impact. 3. Address privacy and security concerns with clear compliance strategies.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Alt-Era</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>D:\hackathon-evaluation\hackathon-evaluation\project_context\ppt\Alt-Era - KRISH PATHAK.pdf</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>6</v>
+      </c>
+      <c r="E7" t="n">
         <v>7</v>
       </c>
-      <c r="G6" t="n">
-        <v>5</v>
-      </c>
-      <c r="H6" t="n">
-        <v>6</v>
-      </c>
-      <c r="I6" t="n">
+      <c r="F7" t="n">
+        <v>7</v>
+      </c>
+      <c r="G7" t="n">
+        <v>4</v>
+      </c>
+      <c r="H7" t="n">
+        <v>6</v>
+      </c>
+      <c r="I7" t="n">
         <v>8</v>
       </c>
-      <c r="J6" t="n">
-        <v>37</v>
-      </c>
-      <c r="K6" t="n">
-        <v>61.5</v>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>The proposal outlines a digital solution for Panchakarma patient management, addressing a growing market need. However, it lacks detailed metrics, clear baselines, and comprehensive evaluation plans. The technical approach is adequate but does not provide sufficient evidence of scalability or risk mitigation strategies.</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>No relevant workflow diagrams were provided; the images included were logos and decorative elements.</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>1. The problem statement is well-framed, highlighting the need for digital tools in the Ayurveda sector. 2. The proposed solution addresses key pain points in patient management effectively.</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>1. The absence of diagrams or detailed workflows limits the understanding of the system architecture and process flow. 2. The proposal lacks specific metrics and KPIs to measure success.</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>1. The choice of technologies is appropriate for the proposed solution, but more detail on integration and scalability is needed. 2. The feasibility section mentions challenges but does not provide a robust mitigation plan.</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>1. Include detailed diagrams to illustrate the system architecture and user workflows. 2. Define clear metrics and KPIs for evaluating the success of the implementation. 3. Address potential risks with a more comprehensive mitigation strategy.</t>
+      <c r="J7" t="n">
+        <v>38</v>
+      </c>
+      <c r="K7" t="n">
+        <v>64</v>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Alt-Era presents a solution for early detection of water-borne diseases using a mobile app and SMS-based platform integrated with IoT and AI/ML technologies. The solution is innovative in its combination of health and water data for outbreak prediction, and it is designed to work in low-bandwidth environments with multilingual support. However, the deck lacks detailed baselines, datasets, and privacy/security considerations. The architecture is well-defined, but cost and latency estimates are missing.</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>No diagrams were provided, so the workflow analysis is based solely on the text description. The proposed workflow involves data collection through mobile apps, SMS, and IoT sensors, followed by AI/ML-driven data processing for outbreak detection and notification to officials and communities.</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>1. The solution is innovative, combining health and water data with AI/ML for early outbreak prediction. 2. The platform is designed to work in low-bandwidth and offline environments, which is crucial for rural areas. 3. Multilingual support enhances accessibility for tribal communities.</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>1. The deck lacks diagrams, which makes it difficult to visualize the architecture and workflow. 2. There is insufficient detail on baselines and datasets used for AI/ML models. 3. Privacy and security considerations are not addressed in the deck.</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>1. The use of low-cost IoT sensors and existing ASHA workforce is a practical approach to data collection. 2. The backend technologies (Django/Node.js) and AI/ML frameworks (TensorFlow, Scikit-learn) are appropriate for the solution.</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>1. Include diagrams to illustrate the architecture and data flow. 2. Provide more details on the datasets and baselines for AI/ML models. 3. Address privacy and security concerns, especially given the sensitive nature of health data.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Angaari Paltan</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>D:\hackathon-evaluation\hackathon-evaluation\project_context\ppt\Angaari Paltan - ISHITA GOYAL.pdf</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>6</v>
+      </c>
+      <c r="E8" t="n">
+        <v>6</v>
+      </c>
+      <c r="F8" t="n">
+        <v>7</v>
+      </c>
+      <c r="G8" t="n">
+        <v>5</v>
+      </c>
+      <c r="H8" t="n">
+        <v>6</v>
+      </c>
+      <c r="I8" t="n">
+        <v>8</v>
+      </c>
+      <c r="J8" t="n">
+        <v>38</v>
+      </c>
+      <c r="K8" t="n">
+        <v>63.5</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>The team 'Angaari Paltan' presented an AI-driven internship recommendation engine aimed at matching user profiles with verified internships. The solution leverages NLP for profile analysis and a hybrid model for matching. However, the presentation lacks diagrams, making it difficult to fully assess the technical architecture and workflow. The problem framing and datasets are adequately covered, but there are significant gaps in assumptions, baselines, and metrics. The deployment plan and adoption path are mentioned but not detailed. Overall, the project shows potential but requires more concrete evidence and detailed planning.</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>No diagrams were provided, so the workflow analysis is based solely on the text description. The workflow involves data collection from verified sources, user profiling using NLP, and a recommendation engine that uses a hybrid model for matching. The deployment includes a web dashboard for ministries and organizations.</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>1. The project addresses a relevant problem in the education sector by facilitating access to internships. 2. The use of NLP for profile analysis is a strong technical choice that can enhance the personalization of recommendations.</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>1. The lack of diagrams makes it difficult to assess the technical architecture and workflow. 2. There is insufficient detail on the assumptions and baselines, which are critical for evaluating the feasibility of the solution.</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>1. The hybrid model combining collaborative filtering and skill matching is a promising approach, but more details on its implementation and evaluation are needed. 2. The data quality challenges are acknowledged, but the proposed strategies for verification and feedback loops require further elaboration.</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>1. Include detailed diagrams to illustrate the architecture and workflow, which will strengthen the technical evaluation. 2. Provide more information on the metrics and evaluation plan to demonstrate how the solution's effectiveness will be measured. 3. Clarify the assumptions and baselines to provide a clearer context for the solution's development and deployment.</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Hacktronics</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>D:\hackathon-evaluation\hackathon-evaluation\project_context\ppt\Animal Type Classification - DEVANG SHUKLA.pdf</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>6</v>
+      </c>
+      <c r="E9" t="n">
+        <v>6</v>
+      </c>
+      <c r="F9" t="n">
+        <v>8</v>
+      </c>
+      <c r="G9" t="n">
+        <v>5</v>
+      </c>
+      <c r="H9" t="n">
+        <v>6</v>
+      </c>
+      <c r="I9" t="n">
+        <v>8</v>
+      </c>
+      <c r="J9" t="n">
+        <v>39</v>
+      </c>
+      <c r="K9" t="n">
+        <v>65.5</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Hacktronics presents an AI-driven solution for animal type classification in rural agriculture, leveraging low-cost hardware and AI frameworks. The project is well-framed with a clear problem statement and a strong architectural plan, but lacks detailed baselines, metrics, and privacy considerations. The diagrams support the data flow and market potential, but the text lacks comprehensive evidence for some criteria.</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>The workflow involves capturing data using a camera, processing it on-device, and transmitting it to a mobile device and cloud, supported by market sizing data for deployment scenarios.</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>1. The project addresses a significant problem in rural agriculture with a clear AI-driven solution. 2. The use of low-cost hardware and AI frameworks is well-integrated into the solution, making it feasible for rural deployment.</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>1. The proposal lacks detailed baselines and metrics for evaluating the system's performance. 2. Privacy and security considerations are minimally addressed, which could be a concern for data handling.</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>1. The architecture is well-documented, but the latency and cost estimates are vague. 2. The dataset requirements are mentioned, but specifics on data collection and diversity are lacking.</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>1. Provide more detailed metrics and evaluation plans to strengthen the proposal. 2. Address privacy and security concerns more thoroughly to ensure data protection. 3. Include more detailed deployment and adoption strategies to enhance the project's feasibility.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>BenzeneCoder</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>D:\hackathon-evaluation\hackathon-evaluation\project_context\ppt\BenzeneCoder - SARTHAK TIWARI.pdf</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>6</v>
+      </c>
+      <c r="E10" t="n">
+        <v>7</v>
+      </c>
+      <c r="F10" t="n">
+        <v>7</v>
+      </c>
+      <c r="G10" t="n">
+        <v>4</v>
+      </c>
+      <c r="H10" t="n">
+        <v>6</v>
+      </c>
+      <c r="I10" t="n">
+        <v>8</v>
+      </c>
+      <c r="J10" t="n">
+        <v>38</v>
+      </c>
+      <c r="K10" t="n">
+        <v>64</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>The team BenzeneCoder presents a digital mental health platform for students, focusing on accessibility and stigma reduction. The solution is technically feasible using open-source tools but lacks detailed metrics, baselines, and deployment plans. Privacy and security are acknowledged but not deeply addressed.</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>The workflow involves developing a web-based platform with core features like AI chatbot, booking system, and resource hub. The process includes defining features, setting up backend and frontend, integrating components, and testing.</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>1. The project addresses a significant issue in student mental health with a proactive approach. 2. The use of open-source tools makes the solution accessible and cost-effective.</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>1. The presentation lacks detailed diagrams to support the technical architecture and workflow. 2. Metrics and evaluation plans are not clearly defined, making it difficult to assess the project's success.</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>1. The integration of AI chatbot with Rasa is a strong point, but the limitations and potential inaccuracies of AI need more robust mitigation strategies. 2. The security measures for handling sensitive data are mentioned but not detailed.</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>1. Include detailed diagrams of the system architecture and data flow to strengthen the technical presentation. 2. Develop a clear evaluation plan with specific metrics to measure the impact and success of the platform. 3. Enhance the privacy and security sections with more specific strategies and technologies.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Binary Brains</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>D:\hackathon-evaluation\hackathon-evaluation\project_context\ppt\Binary Brains - Milan Sharma.pdf</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>5</v>
+      </c>
+      <c r="E11" t="n">
+        <v>6</v>
+      </c>
+      <c r="F11" t="n">
+        <v>6</v>
+      </c>
+      <c r="G11" t="n">
+        <v>4</v>
+      </c>
+      <c r="H11" t="n">
+        <v>5</v>
+      </c>
+      <c r="I11" t="n">
+        <v>7</v>
+      </c>
+      <c r="J11" t="n">
+        <v>33</v>
+      </c>
+      <c r="K11" t="n">
+        <v>55.5</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Binary Brains presents a digital mental health platform for students, leveraging AI for stress detection and personalized support. The proposal is strong in problem framing and architecture, but lacks detailed baselines and dataset information. Privacy and scalability are well-addressed, but metrics and evaluation plans need more clarity.</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>No diagrams or workflows were provided in the deck. The images were primarily logos and decorative elements.</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>1. The problem framing is well-articulated, focusing on a critical issue in student mental health. 2. The proposed solution is innovative, combining AI with human counseling to provide comprehensive support.</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>1. The deck lacks detailed information on datasets and baselines, which are crucial for evaluating the AI model's effectiveness. 2. Metrics and evaluation plans are not clearly defined, making it difficult to assess the project's success criteria.</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>1. The tech stack is well-chosen for scalability and real-time interaction, but more details on latency and cost estimates would strengthen the proposal. 2. Security measures are mentioned, but specifics on how data privacy will be maintained are needed.</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>1. Include detailed baselines and dataset information to strengthen the evidence of feasibility. 2. Define clear metrics and evaluation plans to track the project's impact and success. 3. Provide a more detailed deployment plan, including potential challenges and mitigation strategies.</t>
         </is>
       </c>
     </row>

</xml_diff>